<commit_message>
Fix regression, the hiperparameters of the models was changed. More images in assets was added. Readme update.
</commit_message>
<xml_diff>
--- a/data/output/results/df_class.xlsx
+++ b/data/output/results/df_class.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,6 +844,89 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>9695-TERGH</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Month-to-month</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Electronic check</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>96.05</v>
+      </c>
+      <c r="O6" t="n">
+        <v>431.98</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Betha</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2024-07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>